<commit_message>
Mover canje a usuario en vez de a comercio
Además se cambio la tabla productoXUsuario a Canjes, y se le agregó un atributo de cantidad. También incluí los casos de prueba
</commit_message>
<xml_diff>
--- a/Documentación/Casos de prueba.xlsx
+++ b/Documentación/Casos de prueba.xlsx
@@ -706,8 +706,8 @@
   </sheetPr>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -993,10 +993,10 @@
         <v>12</v>
       </c>
       <c r="D18" s="12"/>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
-      <c r="F18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="2">
@@ -1009,10 +1009,10 @@
         <v>35</v>
       </c>
       <c r="D19" s="12"/>
-      <c r="E19" s="12">
-        <v>1</v>
-      </c>
-      <c r="F19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="2">
@@ -1184,11 +1184,11 @@
       <c r="C30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="12">
-        <v>1</v>
-      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
+      <c r="F30" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="2">
@@ -1200,11 +1200,11 @@
       <c r="C31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="12">
-        <v>1</v>
-      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="F31" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="2">
@@ -1216,11 +1216,11 @@
       <c r="C32" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="12">
-        <v>1</v>
-      </c>
+      <c r="D32" s="12"/>
       <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
+      <c r="F32" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="16">
@@ -1409,10 +1409,10 @@
         <v>80</v>
       </c>
       <c r="D44" s="14"/>
-      <c r="E44" s="12">
-        <v>1</v>
-      </c>
-      <c r="F44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="13.2">
       <c r="A45" s="16">
@@ -1558,15 +1558,15 @@
       </c>
       <c r="D55" s="5">
         <f t="shared" ref="D55:F55" si="0">SUM(D3:D54)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E55">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G55" s="1">
         <v>50</v>

</xml_diff>